<commit_message>
1. users->admin. entities Complite. Next views ...
</commit_message>
<xml_diff>
--- a/docs/Таблицы.xlsx
+++ b/docs/Таблицы.xlsx
@@ -1150,7 +1150,7 @@
   <dimension ref="A3:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1180,7 +1180,7 @@
       <c r="A5" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>85</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -1191,10 +1191,10 @@
       <c r="A6" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="6" t="s">
         <v>55</v>
       </c>
       <c r="D6" t="s">
@@ -1219,10 +1219,10 @@
       <c r="A8" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="6" t="s">
         <v>59</v>
       </c>
       <c r="D8" t="s">
@@ -1348,5 +1348,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2. Admin Cabinet, begin
</commit_message>
<xml_diff>
--- a/docs/Таблицы.xlsx
+++ b/docs/Таблицы.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Таблицы" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="113">
   <si>
     <t>-&gt; User</t>
   </si>
@@ -166,9 +166,6 @@
     <t>2.</t>
   </si>
   <si>
-    <t>booking_users</t>
-  </si>
-  <si>
     <t>3.</t>
   </si>
   <si>
@@ -220,18 +217,9 @@
     <t>users_networks</t>
   </si>
   <si>
-    <t>booking_users_personal</t>
-  </si>
-  <si>
-    <t>booking_users_account</t>
-  </si>
-  <si>
     <t>счета</t>
   </si>
   <si>
-    <t>booking_users_legal</t>
-  </si>
-  <si>
     <t>Сведения об организации (ИНН, ОГРН) или физ.лице (Паспортные данные)</t>
   </si>
   <si>
@@ -292,12 +280,6 @@
     <t>Users</t>
   </si>
   <si>
-    <t>BookingUsers</t>
-  </si>
-  <si>
-    <t>OfficeUsers</t>
-  </si>
-  <si>
     <t>1)</t>
   </si>
   <si>
@@ -374,6 +356,21 @@
   </si>
   <si>
     <t>Smoking, currenty, язык</t>
+  </si>
+  <si>
+    <t>admin\Users</t>
+  </si>
+  <si>
+    <t>office\Users</t>
+  </si>
+  <si>
+    <t>admin_users_personal</t>
+  </si>
+  <si>
+    <t>admin_users_account</t>
+  </si>
+  <si>
+    <t>admin_users_legal</t>
   </si>
 </sst>
 </file>
@@ -458,10 +455,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -744,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:D81"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,10 +755,10 @@
   <sheetData>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -828,7 +825,7 @@
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
         <v>30</v>
@@ -968,41 +965,41 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" t="s">
         <v>56</v>
-      </c>
-      <c r="C49" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
+        <v>58</v>
+      </c>
+      <c r="C50" t="s">
         <v>59</v>
-      </c>
-      <c r="C50" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1010,49 +1007,49 @@
         <v>43</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C54" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B55" s="7" t="s">
+      <c r="B55" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C55" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B56" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C56" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C57" t="s">
         <v>62</v>
-      </c>
-      <c r="C55" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B56" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C56" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B57" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C57" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1062,81 +1059,81 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="C63" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B64" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" s="6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1149,8 +1146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,127 +1162,127 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>88</v>
+      <c r="A5" s="7" t="s">
+        <v>82</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" t="s">
         <v>108</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="B7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" t="s">
         <v>109</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B10" t="s">
-        <v>87</v>
-      </c>
-      <c r="C10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>92</v>
-      </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>93</v>
+      <c r="A12" s="7" t="s">
+        <v>87</v>
       </c>
       <c r="B12" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1293,23 +1290,23 @@
         <v>2</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>88</v>
+      <c r="A17" s="7" t="s">
+        <v>82</v>
       </c>
       <c r="B17" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>89</v>
+      <c r="A18" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="B18" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1317,33 +1314,33 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>88</v>
+      <c r="A23" s="7" t="s">
+        <v>82</v>
       </c>
       <c r="B23" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>89</v>
+      <c r="A24" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="B24" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
-        <v>90</v>
+      <c r="A25" s="7" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3. Entities Stays & Rooms ++ Comfort
</commit_message>
<xml_diff>
--- a/docs/Таблицы.xlsx
+++ b/docs/Таблицы.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="125">
   <si>
     <t>-&gt; User</t>
   </si>
@@ -220,9 +220,6 @@
     <t>счета</t>
   </si>
   <si>
-    <t>Сведения об организации (ИНН, ОГРН) или физ.лице (Паспортные данные)</t>
-  </si>
-  <si>
     <t>персональные данные (ФИО, тел, должность, фото/логотип представителя)</t>
   </si>
   <si>
@@ -370,19 +367,66 @@
     <t>admin_users_account</t>
   </si>
   <si>
-    <t>admin_users_legal</t>
+    <t>admin_users_legals</t>
+  </si>
+  <si>
+    <t>Мои организации: Сведения об организации (Наименование, ИНН, ОГРН) или физ.лице (Ф.И.О.)</t>
+  </si>
+  <si>
+    <t>legal_id</t>
+  </si>
+  <si>
+    <t>Правила</t>
+  </si>
+  <si>
+    <t>1. Отмена, Предоплата</t>
+  </si>
+  <si>
+    <t>2. Размещение детей</t>
+  </si>
+  <si>
+    <t>сколько бесплатно, с какого возраста, или какая сумма</t>
+  </si>
+  <si>
+    <t>3. Доп.кровати</t>
+  </si>
+  <si>
+    <t>Сколько и в какую цену, для детей с какого по какой возраст</t>
+  </si>
+  <si>
+    <t>4. Время заезда</t>
+  </si>
+  <si>
+    <t>5. Интернет</t>
+  </si>
+  <si>
+    <t>да/нет, платно/бесплатно, где(номера, весь отель, общ.места)</t>
+  </si>
+  <si>
+    <t>6.Животные</t>
+  </si>
+  <si>
+    <t>да/нет, платно/бесплатно</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -445,20 +489,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -739,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:D81"/>
+  <dimension ref="A4:D88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,19 +805,19 @@
   <sheetData>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="11" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="11" t="s">
         <v>1</v>
       </c>
     </row>
@@ -788,17 +838,17 @@
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="11" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="11" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="11" t="s">
         <v>8</v>
       </c>
     </row>
@@ -823,317 +873,372 @@
         <v>19</v>
       </c>
     </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>115</v>
+      </c>
+    </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
-        <v>65</v>
+      <c r="B18" t="s">
+        <v>116</v>
       </c>
       <c r="C18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>123</v>
+      </c>
+      <c r="C22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C27" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C28" s="5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C36" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C30" s="5" t="s">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C31" s="5" t="s">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="6" t="s">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C45" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>33</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C46" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
         <v>35</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C47" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>40</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C46" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>54</v>
-      </c>
-      <c r="C48" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>40</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C53" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B54" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>54</v>
+      </c>
+      <c r="C55" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
         <v>55</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C56" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
         <v>58</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C57" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>43</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C54" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B55" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="C55" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B56" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="C56" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B57" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="C57" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>43</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C61" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B62" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C62" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B63" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C63" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>44</v>
       </c>
-      <c r="B63" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C63" t="s">
+      <c r="B70" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C70" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B64" s="5" t="s">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B71" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="6" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B77" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>76</v>
+      </c>
+      <c r="C88" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1162,23 +1267,23 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>41</v>
@@ -1186,52 +1291,52 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C7" t="s">
         <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C9" t="s">
         <v>45</v>
@@ -1239,18 +1344,18 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B11" t="s">
         <v>47</v>
@@ -1261,10 +1366,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" t="s">
         <v>87</v>
-      </c>
-      <c r="B12" t="s">
-        <v>88</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>60</v>
@@ -1272,17 +1377,17 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1290,23 +1395,23 @@
         <v>2</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1314,17 +1419,17 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B23" t="s">
         <v>31</v>
@@ -1332,15 +1437,15 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3. Entities Stays & Rooms ++ Comfort, Rules++
</commit_message>
<xml_diff>
--- a/docs/Таблицы.xlsx
+++ b/docs/Таблицы.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Таблицы" sheetId="1" r:id="rId1"/>
     <sheet name="Этапность" sheetId="2" r:id="rId2"/>
+    <sheet name="Классы" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="132">
   <si>
     <t>-&gt; User</t>
   </si>
@@ -408,12 +409,33 @@
   <si>
     <t>да/нет, платно/бесплатно</t>
   </si>
+  <si>
+    <t>Comfort</t>
+  </si>
+  <si>
+    <t>manage\</t>
+  </si>
+  <si>
+    <t>Сервисы</t>
+  </si>
+  <si>
+    <t>то, что будет редактироваться в office</t>
+  </si>
+  <si>
+    <t>Rules</t>
+  </si>
+  <si>
+    <t>Comfort (Stays)</t>
+  </si>
+  <si>
+    <t>Comfort (Rooms)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -462,6 +484,13 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -489,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
@@ -509,6 +538,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -791,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:D88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,12 +916,12 @@
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>116</v>
       </c>
@@ -899,7 +929,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>118</v>
       </c>
@@ -907,28 +937,31 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>125</v>
+      </c>
+      <c r="B21" s="13" t="s">
         <v>121</v>
       </c>
       <c r="C21" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="13" t="s">
         <v>123</v>
       </c>
       <c r="C22" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
         <v>64</v>
       </c>
@@ -936,17 +969,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>12</v>
       </c>
@@ -954,7 +987,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>14</v>
       </c>
@@ -962,17 +995,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>18</v>
       </c>
@@ -1452,4 +1485,47 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
3. Entities Stays & Rooms ++ Comfort, Rules+++ Tours
</commit_message>
<xml_diff>
--- a/docs/Таблицы.xlsx
+++ b/docs/Таблицы.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="136">
   <si>
     <t>-&gt; User</t>
   </si>
@@ -429,6 +429,18 @@
   </si>
   <si>
     <t>Comfort (Rooms)</t>
+  </si>
+  <si>
+    <t>admin_user_personal</t>
+  </si>
+  <si>
+    <t>admin_user_legals</t>
+  </si>
+  <si>
+    <t>В рамках UserService</t>
+  </si>
+  <si>
+    <t>UserLegalService+Repository</t>
   </si>
 </sst>
 </file>
@@ -1282,16 +1294,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D25"/>
+  <dimension ref="A3:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
     <col min="4" max="4" width="61.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1376,108 +1388,126 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B10" t="s">
-        <v>108</v>
-      </c>
-      <c r="C10" t="s">
-        <v>79</v>
+      <c r="A10" s="7"/>
+      <c r="C10" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D10" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" t="s">
-        <v>38</v>
+      <c r="A11" s="7"/>
+      <c r="C11" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D11" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>87</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C14" s="6" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
         <v>2</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B18" s="6" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B19" s="6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>3</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B23" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B24" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>

<commit_message>
4. AdminUser Finance +++ DatePicker!++
</commit_message>
<xml_diff>
--- a/docs/Таблицы.xlsx
+++ b/docs/Таблицы.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Таблицы" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="133">
   <si>
     <t>-&gt; User</t>
   </si>
@@ -218,9 +218,6 @@
     <t>users_networks</t>
   </si>
   <si>
-    <t>счета</t>
-  </si>
-  <si>
     <t>персональные данные (ФИО, тел, должность, фото/логотип представителя)</t>
   </si>
   <si>
@@ -233,36 +230,6 @@
     <t>Address</t>
   </si>
   <si>
-    <t>Страна</t>
-  </si>
-  <si>
-    <t>Город</t>
-  </si>
-  <si>
-    <t>Улица</t>
-  </si>
-  <si>
-    <t>Индекс</t>
-  </si>
-  <si>
-    <t>Регион</t>
-  </si>
-  <si>
-    <t>Нас.пункт</t>
-  </si>
-  <si>
-    <t>Район</t>
-  </si>
-  <si>
-    <t>Дом</t>
-  </si>
-  <si>
-    <t>Корпус</t>
-  </si>
-  <si>
-    <t>Квартира</t>
-  </si>
-  <si>
     <t>Геолокация</t>
   </si>
   <si>
@@ -365,9 +332,6 @@
     <t>admin_users_personal</t>
   </si>
   <si>
-    <t>admin_users_account</t>
-  </si>
-  <si>
     <t>admin_users_legals</t>
   </si>
   <si>
@@ -441,6 +405,33 @@
   </si>
   <si>
     <t>UserLegalService+Repository</t>
+  </si>
+  <si>
+    <t>Строка адреса</t>
+  </si>
+  <si>
+    <t>Форум для партнеров</t>
+  </si>
+  <si>
+    <t>5.</t>
+  </si>
+  <si>
+    <t>InfoPlace</t>
+  </si>
+  <si>
+    <t>Реклама разных объектов /Питание, Магазины (сувен.)</t>
+  </si>
+  <si>
+    <t>6.</t>
+  </si>
+  <si>
+    <t>7.</t>
+  </si>
+  <si>
+    <t>Блог</t>
+  </si>
+  <si>
+    <t>8.</t>
   </si>
 </sst>
 </file>
@@ -530,7 +521,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
@@ -544,13 +535,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -831,39 +825,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:D88"/>
+  <dimension ref="A4:D116"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.140625" style="14"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
     <col min="3" max="3" width="43.28515625" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
     <col min="7" max="7" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>40</v>
+      </c>
       <c r="B4" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
@@ -874,27 +872,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
@@ -902,7 +900,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
@@ -910,84 +908,84 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="9" t="s">
-        <v>113</v>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
+        <v>101</v>
       </c>
       <c r="C15" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="C18" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="C19" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>125</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>121</v>
+      <c r="A21" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>109</v>
       </c>
       <c r="C21" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="13" t="s">
-        <v>123</v>
+      <c r="B22" s="12" t="s">
+        <v>111</v>
       </c>
       <c r="C22" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C25" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="11" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1022,7 +1020,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>21</v>
       </c>
@@ -1030,17 +1028,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C34" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C35" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>25</v>
       </c>
@@ -1048,242 +1046,280 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C37" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C38" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="4" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="6"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B54" s="6"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="6"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="14">
+        <v>4</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="6"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B58" s="6"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="6"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C60" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B61" s="6"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B62" s="6"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B63" s="6"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B65" s="6"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="6"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="6"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C86" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B87" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>54</v>
+      </c>
+      <c r="C88" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>55</v>
+      </c>
+      <c r="C89" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>58</v>
+      </c>
+      <c r="C90" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B94" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="6" t="s">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B95" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C95" s="13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
         <v>33</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C96" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B97" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C97" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>40</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C53" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B54" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>54</v>
-      </c>
-      <c r="C55" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>55</v>
-      </c>
-      <c r="C56" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>58</v>
-      </c>
-      <c r="C57" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>43</v>
-      </c>
-      <c r="B61" s="6" t="s">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B102" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C102" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B62" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="C62" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B63" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="C63" t="s">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B103" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C103" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C64" s="10" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
+    <row r="104" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="14"/>
+      <c r="B104" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C104" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>44</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C70" t="s">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B110" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C110" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B71" s="5" t="s">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B111" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B77" s="6" t="s">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B114" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
+      <c r="C116" s="1" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B87" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
-        <v>76</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1312,23 +1348,23 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>41</v>
@@ -1336,52 +1372,52 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
         <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="C9" t="s">
         <v>45</v>
@@ -1390,35 +1426,35 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="C10" s="6" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="D10" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="C11" s="6" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="D11" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C12" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
         <v>47</v>
@@ -1429,10 +1465,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>60</v>
@@ -1440,17 +1476,17 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1458,23 +1494,23 @@
         <v>2</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" t="s">
         <v>82</v>
-      </c>
-      <c r="B20" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1482,17 +1518,17 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B25" t="s">
         <v>31</v>
@@ -1500,15 +1536,15 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="B26" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1521,7 +1557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1529,30 +1565,30 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="C3" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
7. User Admin Notice (Service begin +
</commit_message>
<xml_diff>
--- a/docs/Таблицы.xlsx
+++ b/docs/Таблицы.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="161">
   <si>
     <t>-&gt; User</t>
   </si>
@@ -952,8 +952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1255,14 +1255,11 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+      <c r="B45" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="C45" s="23" t="s">
         <v>154</v>
-      </c>
-      <c r="D45" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1572,8 +1569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:E31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:D13"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>